<commit_message>
Updated merge Invoice/DataTreatment xaml.
</commit_message>
<xml_diff>
--- a/Input/purchase_plan_18_7_2025.xlsx
+++ b/Input/purchase_plan_18_7_2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9cac9347e88df44a/Área de Trabalho/Projetos TCS/Desafio Final/Desafio-Final-Robot/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Documents\UiPath\Desafio_Final_TCS\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{8FD831D6-D63F-42D6-BECB-369AF65AC3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81ABDC58-8305-4429-9AA8-B65867894C67}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5DF622-03E9-4495-B63E-1FB33433C760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" xr2:uid="{53D26817-BE4F-4DAB-BE4A-38A456060AB0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{53D26817-BE4F-4DAB-BE4A-38A456060AB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -112,7 +110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,9 +479,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,7 +519,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>748</v>
       </c>
@@ -559,7 +557,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>748</v>
       </c>
@@ -597,7 +595,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>6</v>
       </c>
@@ -635,7 +633,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>6</v>
       </c>
@@ -684,7 +682,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>